<commit_message>
commit intermediate problem solution
</commit_message>
<xml_diff>
--- a/outputs/BatchCustomerMapping.xlsx
+++ b/outputs/BatchCustomerMapping.xlsx
@@ -340,15 +340,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:X24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:24">
       <c r="A1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1">
         <v>0</v>
@@ -371,10 +371,58 @@
       <c r="H1">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="I1">
+        <v>0</v>
+      </c>
+      <c r="J1">
+        <v>0</v>
+      </c>
+      <c r="K1">
+        <v>0</v>
+      </c>
+      <c r="L1">
+        <v>1</v>
+      </c>
+      <c r="M1">
+        <v>0</v>
+      </c>
+      <c r="N1">
+        <v>0</v>
+      </c>
+      <c r="O1">
+        <v>0</v>
+      </c>
+      <c r="P1">
+        <v>0</v>
+      </c>
+      <c r="Q1">
+        <v>0</v>
+      </c>
+      <c r="R1">
+        <v>0</v>
+      </c>
+      <c r="S1">
+        <v>0</v>
+      </c>
+      <c r="T1">
+        <v>0</v>
+      </c>
+      <c r="U1">
+        <v>0</v>
+      </c>
+      <c r="V1">
+        <v>0</v>
+      </c>
+      <c r="W1">
+        <v>0</v>
+      </c>
+      <c r="X1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24">
       <c r="A2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -389,7 +437,7 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -397,8 +445,56 @@
       <c r="H2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24">
       <c r="A3">
         <v>0</v>
       </c>
@@ -409,7 +505,7 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -423,8 +519,56 @@
       <c r="H3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>0</v>
+      </c>
+      <c r="X3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24">
       <c r="A4">
         <v>0</v>
       </c>
@@ -435,7 +579,7 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -449,10 +593,58 @@
       <c r="H4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+      <c r="X4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24">
       <c r="A5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -475,8 +667,56 @@
       <c r="H5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+      <c r="X5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24">
       <c r="A6">
         <v>0</v>
       </c>
@@ -499,12 +739,60 @@
         <v>0</v>
       </c>
       <c r="H6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <v>1</v>
+      </c>
+      <c r="W6">
+        <v>0</v>
+      </c>
+      <c r="X6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24">
       <c r="A7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -527,8 +815,56 @@
       <c r="H7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <v>1</v>
+      </c>
+      <c r="X7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24">
       <c r="A8">
         <v>0</v>
       </c>
@@ -551,7 +887,1239 @@
         <v>0</v>
       </c>
       <c r="H8">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8">
+        <v>0</v>
+      </c>
+      <c r="U8">
+        <v>0</v>
+      </c>
+      <c r="V8">
+        <v>0</v>
+      </c>
+      <c r="W8">
+        <v>0</v>
+      </c>
+      <c r="X8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24">
+      <c r="A9">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>1</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <v>0</v>
+      </c>
+      <c r="U9">
+        <v>0</v>
+      </c>
+      <c r="V9">
+        <v>0</v>
+      </c>
+      <c r="W9">
+        <v>0</v>
+      </c>
+      <c r="X9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>1</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>0</v>
+      </c>
+      <c r="T10">
+        <v>0</v>
+      </c>
+      <c r="U10">
+        <v>0</v>
+      </c>
+      <c r="V10">
+        <v>0</v>
+      </c>
+      <c r="W10">
+        <v>0</v>
+      </c>
+      <c r="X10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24">
+      <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>1</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="T11">
+        <v>0</v>
+      </c>
+      <c r="U11">
+        <v>0</v>
+      </c>
+      <c r="V11">
+        <v>0</v>
+      </c>
+      <c r="W11">
+        <v>0</v>
+      </c>
+      <c r="X11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24">
+      <c r="A12">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>0</v>
+      </c>
+      <c r="S12">
+        <v>0</v>
+      </c>
+      <c r="T12">
+        <v>0</v>
+      </c>
+      <c r="U12">
+        <v>0</v>
+      </c>
+      <c r="V12">
+        <v>0</v>
+      </c>
+      <c r="W12">
+        <v>0</v>
+      </c>
+      <c r="X12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24">
+      <c r="A13">
+        <v>0</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>1</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <v>0</v>
+      </c>
+      <c r="T13">
+        <v>0</v>
+      </c>
+      <c r="U13">
+        <v>0</v>
+      </c>
+      <c r="V13">
+        <v>0</v>
+      </c>
+      <c r="W13">
+        <v>0</v>
+      </c>
+      <c r="X13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24">
+      <c r="A14">
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <v>0</v>
+      </c>
+      <c r="T14">
+        <v>0</v>
+      </c>
+      <c r="U14">
+        <v>1</v>
+      </c>
+      <c r="V14">
+        <v>0</v>
+      </c>
+      <c r="W14">
+        <v>0</v>
+      </c>
+      <c r="X14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24">
+      <c r="A15">
+        <v>0</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>1</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
+      <c r="T15">
+        <v>0</v>
+      </c>
+      <c r="U15">
+        <v>0</v>
+      </c>
+      <c r="V15">
+        <v>0</v>
+      </c>
+      <c r="W15">
+        <v>0</v>
+      </c>
+      <c r="X15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24">
+      <c r="A16">
+        <v>0</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+      <c r="R16">
+        <v>0</v>
+      </c>
+      <c r="S16">
+        <v>0</v>
+      </c>
+      <c r="T16">
+        <v>0</v>
+      </c>
+      <c r="U16">
+        <v>0</v>
+      </c>
+      <c r="V16">
+        <v>0</v>
+      </c>
+      <c r="W16">
+        <v>0</v>
+      </c>
+      <c r="X16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24">
+      <c r="A17">
+        <v>0</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>1</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <v>0</v>
+      </c>
+      <c r="S17">
+        <v>0</v>
+      </c>
+      <c r="T17">
+        <v>0</v>
+      </c>
+      <c r="U17">
+        <v>0</v>
+      </c>
+      <c r="V17">
+        <v>0</v>
+      </c>
+      <c r="W17">
+        <v>0</v>
+      </c>
+      <c r="X17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24">
+      <c r="A18">
+        <v>0</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18">
+        <v>1</v>
+      </c>
+      <c r="Q18">
+        <v>0</v>
+      </c>
+      <c r="R18">
+        <v>0</v>
+      </c>
+      <c r="S18">
+        <v>0</v>
+      </c>
+      <c r="T18">
+        <v>0</v>
+      </c>
+      <c r="U18">
+        <v>0</v>
+      </c>
+      <c r="V18">
+        <v>0</v>
+      </c>
+      <c r="W18">
+        <v>0</v>
+      </c>
+      <c r="X18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24">
+      <c r="A19">
+        <v>0</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>1</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="Q19">
+        <v>0</v>
+      </c>
+      <c r="R19">
+        <v>0</v>
+      </c>
+      <c r="S19">
+        <v>0</v>
+      </c>
+      <c r="T19">
+        <v>0</v>
+      </c>
+      <c r="U19">
+        <v>0</v>
+      </c>
+      <c r="V19">
+        <v>0</v>
+      </c>
+      <c r="W19">
+        <v>0</v>
+      </c>
+      <c r="X19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24">
+      <c r="A20">
+        <v>0</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20">
+        <v>0</v>
+      </c>
+      <c r="Q20">
+        <v>0</v>
+      </c>
+      <c r="R20">
+        <v>0</v>
+      </c>
+      <c r="S20">
+        <v>0</v>
+      </c>
+      <c r="T20">
+        <v>0</v>
+      </c>
+      <c r="U20">
+        <v>0</v>
+      </c>
+      <c r="V20">
+        <v>0</v>
+      </c>
+      <c r="W20">
+        <v>1</v>
+      </c>
+      <c r="X20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24">
+      <c r="A21">
+        <v>0</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>1</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <v>0</v>
+      </c>
+      <c r="R21">
+        <v>0</v>
+      </c>
+      <c r="S21">
+        <v>0</v>
+      </c>
+      <c r="T21">
+        <v>0</v>
+      </c>
+      <c r="U21">
+        <v>0</v>
+      </c>
+      <c r="V21">
+        <v>0</v>
+      </c>
+      <c r="W21">
+        <v>0</v>
+      </c>
+      <c r="X21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="P22">
+        <v>0</v>
+      </c>
+      <c r="Q22">
+        <v>0</v>
+      </c>
+      <c r="R22">
+        <v>0</v>
+      </c>
+      <c r="S22">
+        <v>0</v>
+      </c>
+      <c r="T22">
+        <v>0</v>
+      </c>
+      <c r="U22">
+        <v>0</v>
+      </c>
+      <c r="V22">
+        <v>0</v>
+      </c>
+      <c r="W22">
+        <v>0</v>
+      </c>
+      <c r="X22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24">
+      <c r="A23">
+        <v>0</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="P23">
+        <v>1</v>
+      </c>
+      <c r="Q23">
+        <v>0</v>
+      </c>
+      <c r="R23">
+        <v>0</v>
+      </c>
+      <c r="S23">
+        <v>0</v>
+      </c>
+      <c r="T23">
+        <v>0</v>
+      </c>
+      <c r="U23">
+        <v>0</v>
+      </c>
+      <c r="V23">
+        <v>0</v>
+      </c>
+      <c r="W23">
+        <v>0</v>
+      </c>
+      <c r="X23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24">
+      <c r="A24">
+        <v>0</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="O24">
+        <v>0</v>
+      </c>
+      <c r="P24">
+        <v>0</v>
+      </c>
+      <c r="Q24">
+        <v>0</v>
+      </c>
+      <c r="R24">
+        <v>0</v>
+      </c>
+      <c r="S24">
+        <v>0</v>
+      </c>
+      <c r="T24">
+        <v>0</v>
+      </c>
+      <c r="U24">
+        <v>0</v>
+      </c>
+      <c r="V24">
+        <v>0</v>
+      </c>
+      <c r="W24">
+        <v>0</v>
+      </c>
+      <c r="X24">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>